<commit_message>
Changes in git file
</commit_message>
<xml_diff>
--- a/Git Commands.xlsx
+++ b/Git Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shivam\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724FF0A5-9094-488A-9F27-860F8A9709A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78986C3-C16C-4942-9D1E-1527A5BA79D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -306,9 +306,6 @@
   </si>
   <si>
     <t>git add &lt;path&gt;</t>
-  </si>
-  <si>
-    <t>Stage a specific directory or file</t>
   </si>
   <si>
     <t>Stage all files (that are not listed in the .gitignore) in the entire repository</t>
@@ -525,6 +522,12 @@
   <si>
     <t>git stash pop
 git stash pop index</t>
+  </si>
+  <si>
+    <t>The git add command adds a change in the working directory to the staging area.
+It tells Git that you want to include updates to a particular file in the next commit.
+However, git add doesn't really affect the repository in any significant way—changes are not actually recorded until you run git commit.
+Stage a specific directory or file.</t>
   </si>
 </sst>
 </file>
@@ -778,7 +781,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -876,28 +879,31 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1184,7 +1190,7 @@
   <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" zoomScale="105" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1194,10 +1200,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="42"/>
     </row>
     <row r="4" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1333,7 +1339,7 @@
     </row>
     <row r="24" spans="1:2" ht="26" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>23</v>
@@ -1449,26 +1455,26 @@
     </row>
     <row r="40" spans="1:2" ht="52" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="26" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="26" x14ac:dyDescent="0.35">
       <c r="A42" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -1502,12 +1508,12 @@
       <c r="A47" s="23"/>
       <c r="B47" s="13"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" ht="52" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="29" t="s">
-        <v>67</v>
+      <c r="B48" s="43" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -1515,7 +1521,7 @@
         <v>65</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -1524,18 +1530,18 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -1544,18 +1550,18 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="16" t="s">
         <v>75</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -1563,75 +1569,75 @@
       <c r="B56" s="11"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="36" t="s">
+      <c r="A57" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="B57" s="37" t="s">
+    </row>
+    <row r="58" spans="1:2" ht="26" x14ac:dyDescent="0.35">
+      <c r="A58" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B58" s="39" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="35" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" ht="26" x14ac:dyDescent="0.35">
-      <c r="A58" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="B58" s="40" t="s">
+      <c r="B59" s="36" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="36" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="26" x14ac:dyDescent="0.35">
+      <c r="A61" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B61" s="36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="26" x14ac:dyDescent="0.35">
+      <c r="A62" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B59" s="37" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="B60" s="37" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="26" x14ac:dyDescent="0.35">
-      <c r="A61" s="41" t="s">
-        <v>112</v>
-      </c>
-      <c r="B61" s="37" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="26" x14ac:dyDescent="0.35">
-      <c r="A62" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="B62" s="39" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="40" t="s">
+      <c r="B64" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="B63" s="40" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="B64" s="40" t="s">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="39" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="40" t="s">
+      <c r="B65" s="39" t="s">
         <v>110</v>
-      </c>
-      <c r="B65" s="40" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
@@ -1699,50 +1705,50 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B79" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A80" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B80" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B81" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B82" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A83" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B83" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="42" t="s">
+      <c r="A84" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B84" s="41" t="s">
         <v>98</v>
-      </c>
-      <c r="B84" s="42" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>